<commit_message>
Modif oublié de push cost
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/ST/STA0100_to_STA0400.xlsx
+++ b/CR - Cost Report/BOM/ST/STA0100_to_STA0400.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume Touzé\Documents\GitHub\STUF2019\CR - Cost Report\BOM\ST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\ST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6215E2E4-9FA1-404D-93D4-AE2DEEB6A72F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t>System</t>
   </si>
@@ -58,18 +57,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Name of the part</t>
-  </si>
-  <si>
-    <t>m or b</t>
-  </si>
-  <si>
-    <t>Short description of the part</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Part </t>
     </r>
@@ -127,15 +114,9 @@
     <t>b</t>
   </si>
   <si>
-    <t>Tapped insert</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
-    <t>Tapped, glued to carbon tube</t>
-  </si>
-  <si>
     <t>ST_A0100</t>
   </si>
   <si>
@@ -145,36 +126,18 @@
     <t>Spacer</t>
   </si>
   <si>
-    <t>Spacer between the steering whel and the Quick release</t>
-  </si>
-  <si>
     <t>Quick Release mobil part</t>
   </si>
   <si>
-    <t>Removing part of the Quick release.</t>
-  </si>
-  <si>
     <t>Steering shaft</t>
   </si>
   <si>
     <t>ST_A0300</t>
   </si>
   <si>
-    <t>Quick Release Steel Sleeve</t>
-  </si>
-  <si>
-    <t>Fixed part of the Quick release.</t>
-  </si>
-  <si>
     <t>ST_03001</t>
   </si>
   <si>
-    <t>Steering Upper Shaft Pivot</t>
-  </si>
-  <si>
-    <t>Bearing seat for the steering pivot.</t>
-  </si>
-  <si>
     <t>ST_03002</t>
   </si>
   <si>
@@ -187,15 +150,6 @@
     <t>Spline coupler</t>
   </si>
   <si>
-    <t>To connect the steering column to the steering rack.</t>
-  </si>
-  <si>
-    <t>Bearing</t>
-  </si>
-  <si>
-    <t>Steering pivot bearings.</t>
-  </si>
-  <si>
     <t>ST_A0200</t>
   </si>
   <si>
@@ -205,9 +159,6 @@
     <t>ST_02002</t>
   </si>
   <si>
-    <t>U-joint between the steering column and ST_02002.</t>
-  </si>
-  <si>
     <t>ST_02003</t>
   </si>
   <si>
@@ -230,12 +181,84 @@
   </si>
   <si>
     <t>Bought at Formula Seven.</t>
+  </si>
+  <si>
+    <t>Carbon tube</t>
+  </si>
+  <si>
+    <t>Steering Shaft Pivot</t>
+  </si>
+  <si>
+    <t>Tapped insert, right hand</t>
+  </si>
+  <si>
+    <t>Tapped insert, left hand</t>
+  </si>
+  <si>
+    <t>carbon tubes for tie rod</t>
+  </si>
+  <si>
+    <t>Right-hand thread, glued to carbon tube</t>
+  </si>
+  <si>
+    <t>Left-hand thread, glued to carbon tube</t>
+  </si>
+  <si>
+    <t>U-joint for steering column and ST_02002</t>
+  </si>
+  <si>
+    <t>Connect the steering column to the rack</t>
+  </si>
+  <si>
+    <t>2 with a left-hand thread</t>
+  </si>
+  <si>
+    <t>2 with a right-hand thread</t>
+  </si>
+  <si>
+    <t>ST_04007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spacer </t>
+  </si>
+  <si>
+    <t>M6 type 16 mm spacer</t>
+  </si>
+  <si>
+    <t>M6 type 25 mm spacer</t>
+  </si>
+  <si>
+    <t>Rod ends bearing, male r</t>
+  </si>
+  <si>
+    <t>Rod ends bearing, male l</t>
+  </si>
+  <si>
+    <t>Quick Release Shaft</t>
+  </si>
+  <si>
+    <t>Bearing, Ball, Radial</t>
+  </si>
+  <si>
+    <t>Steering pivot bearings</t>
+  </si>
+  <si>
+    <t>Bearing seat for the steering pivot</t>
+  </si>
+  <si>
+    <t>Fixed part of the Quick release</t>
+  </si>
+  <si>
+    <t>Removing part of the Quick release</t>
+  </si>
+  <si>
+    <t>Between steering wheel and Quick release</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -635,21 +658,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.21875" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="44.44140625" customWidth="1"/>
+    <col min="5" max="5" width="41.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" customWidth="1"/>
     <col min="7" max="7" width="16.88671875" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" customWidth="1"/>
@@ -663,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -680,137 +703,137 @@
     </row>
     <row r="2" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>51</v>
@@ -819,246 +842,265 @@
         <v>1</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="F12" s="3">
         <v>2</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F15" s="3">
         <v>4</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>9</v>
+        <v>50</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>9</v>
+        <v>48</v>
+      </c>
+      <c r="F19" s="3">
+        <v>2</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>9</v>
+        <v>53</v>
+      </c>
+      <c r="F20" s="3">
+        <v>2</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>9</v>
+        <v>54</v>
+      </c>
+      <c r="F21" s="3">
+        <v>2</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>9</v>
+        <v>57</v>
+      </c>
+      <c r="F22" s="3">
+        <v>2</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="3">
+        <v>2</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout photo brackets steering + cache-crémaillère
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/ST/STA0100_to_STA0400.xlsx
+++ b/CR - Cost Report/BOM/ST/STA0100_to_STA0400.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\ST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume Touzé\Documents\GitHub\STUF2019\CR - Cost Report\BOM\ST\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C90488-A60C-43E2-830F-43089FDABD20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
   <si>
     <t>System</t>
   </si>
@@ -254,11 +255,20 @@
   <si>
     <t>Between steering wheel and Quick release</t>
   </si>
+  <si>
+    <t>Steering Rack protection</t>
+  </si>
+  <si>
+    <t>To protect the steering rack.</t>
+  </si>
+  <si>
+    <t>ST_03003</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -658,12 +668,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,133 +965,133 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="3">
-        <v>2</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" s="3">
         <v>2</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F19" s="3">
         <v>2</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F20" s="3">
         <v>2</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F21" s="3">
         <v>2</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F22" s="3">
         <v>2</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1094,12 +1104,31 @@
         <v>21</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F23" s="3">
         <v>2</v>
       </c>
       <c r="G23" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="3">
+        <v>2</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>